<commit_message>
added example of how it works
</commit_message>
<xml_diff>
--- a/dsa a-star algorithm.xlsx
+++ b/dsa a-star algorithm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebastiansefort/KEA/dsa/exam-dsa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A61FA8B-072D-C542-8BC7-A66D8DAA5E20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD5ED7DD-1548-074A-84C7-583E63669BE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="760" windowWidth="30240" windowHeight="17780" xr2:uid="{557471D5-42A3-404F-B4E7-C8F59DAE9A90}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17780" xr2:uid="{557471D5-42A3-404F-B4E7-C8F59DAE9A90}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -532,7 +532,7 @@
   <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>